<commit_message>
fixed field name error
</commit_message>
<xml_diff>
--- a/wujian100_sim/reg_model/Excel/wujian100_usi0_reg_spec.xlsx
+++ b/wujian100_sim/reg_model/Excel/wujian100_usi0_reg_spec.xlsx
@@ -387,7 +387,7 @@
     <t xml:space="preserve">[31:1]</t>
   </si>
   <si>
-    <t xml:space="preserve">MS_MDOE</t>
+    <t xml:space="preserve">MS_MODE</t>
   </si>
   <si>
     <t xml:space="preserve">0x0: I2CS mode.
@@ -1268,7 +1268,7 @@
     <numFmt numFmtId="167" formatCode="H:MM"/>
     <numFmt numFmtId="168" formatCode="YYYY\-M\-D\ H:MM"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1325,12 +1325,6 @@
       <name val="宋体"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -1499,7 +1493,7 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1511,15 +1505,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1731,9 +1725,9 @@
   <dimension ref="A1:K180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -1744,7 +1738,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="17.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="6" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="7" width="19.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="17.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="17.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="60.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="33.79"/>
@@ -2524,7 +2518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="22"/>

</xml_diff>

<commit_message>
fixed usi register Excel
</commit_message>
<xml_diff>
--- a/wujian100_sim/reg_model/Excel/wujian100_usi0_reg_spec.xlsx
+++ b/wujian100_sim/reg_model/Excel/wujian100_usi0_reg_spec.xlsx
@@ -1001,7 +1001,7 @@
     <t>0x5C</t>
   </si>
   <si>
-    <t>INTR_MASK</t>
+    <t>INTR_UNMASK</t>
   </si>
   <si>
     <t>SPI_STOP_MASK</t>
@@ -2767,9 +2767,9 @@
   <dimension ref="A1:K180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="D132" sqref="D132:D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>